<commit_message>
- testes dos requisitos do palindromo feitos no excel
</commit_message>
<xml_diff>
--- a/Grafo/doc/casos de teste palindromo.xlsx
+++ b/Grafo/doc/casos de teste palindromo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UFRJ\ProjTesteSoftware\Grafo\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\workspace\ProjTesteSoftware\Grafo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>CT1</t>
   </si>
@@ -267,16 +267,35 @@
   </si>
   <si>
     <t>(10, 7, 8, 10)</t>
+  </si>
+  <si>
+    <t>CT5</t>
+  </si>
+  <si>
+    <t>CT6</t>
+  </si>
+  <si>
+    <t>CT7</t>
+  </si>
+  <si>
+    <t>CT8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -373,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -382,6 +401,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,7 +425,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -720,28 +747,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AB34"/>
+  <dimension ref="B2:AF34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="AF1" sqref="AD1:AF1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" customWidth="1"/>
-    <col min="24" max="24" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" customWidth="1"/>
+    <col min="24" max="24" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="25" max="30" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
@@ -798,9 +827,21 @@
       <c r="AB2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="AC2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2">
@@ -810,7 +851,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -820,17 +861,17 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="P3" s="10" t="s">
+      <c r="P3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
       <c r="U3" s="1"/>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="X3" s="2" t="s">
@@ -838,11 +879,15 @@
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
+      <c r="AA3" s="5"/>
       <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
       <c r="C4" s="2">
         <v>2</v>
       </c>
@@ -850,7 +895,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="I4" s="8"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="2" t="s">
         <v>9</v>
       </c>
@@ -858,25 +903,29 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="1"/>
-      <c r="P4" s="11"/>
+      <c r="P4" s="12"/>
       <c r="Q4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="W4" s="11"/>
+      <c r="U4" s="5"/>
+      <c r="W4" s="12"/>
       <c r="X4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+    </row>
+    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B5" s="7"/>
       <c r="C5" s="2">
         <v>3</v>
       </c>
@@ -884,7 +933,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="1"/>
-      <c r="I5" s="8"/>
+      <c r="I5" s="9"/>
       <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
@@ -892,25 +941,29 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="P5" s="11"/>
+      <c r="P5" s="12"/>
       <c r="Q5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="2" t="s">
+      <c r="W5" s="12"/>
+      <c r="X5" s="16" t="s">
         <v>51</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B6" s="7"/>
       <c r="C6" s="2">
         <v>4</v>
       </c>
@@ -918,7 +971,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="9"/>
       <c r="J6" s="2" t="s">
         <v>11</v>
       </c>
@@ -926,25 +979,29 @@
       <c r="L6" s="5"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="P6" s="11"/>
+      <c r="P6" s="12"/>
       <c r="Q6" s="2" t="s">
         <v>29</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
+      <c r="T6" s="5"/>
       <c r="U6" s="1"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="2" t="s">
+      <c r="W6" s="12"/>
+      <c r="X6" s="16" t="s">
         <v>52</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B7" s="7"/>
       <c r="C7" s="2">
         <v>5</v>
       </c>
@@ -952,7 +1009,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="1"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="2" t="s">
         <v>13</v>
       </c>
@@ -960,25 +1017,29 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="1"/>
-      <c r="P7" s="11"/>
+      <c r="P7" s="12"/>
       <c r="Q7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="2" t="s">
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="16" t="s">
         <v>53</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
       <c r="C8" s="2">
         <v>6</v>
       </c>
@@ -986,7 +1047,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="9"/>
       <c r="J8" s="2" t="s">
         <v>12</v>
       </c>
@@ -994,25 +1055,29 @@
       <c r="L8" s="5"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="P8" s="11"/>
+      <c r="P8" s="12"/>
       <c r="Q8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="W8" s="11"/>
+      <c r="W8" s="12"/>
       <c r="X8" s="2" t="s">
         <v>54</v>
       </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
+      <c r="AB8" s="5"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B9" s="7"/>
       <c r="C9" s="2">
         <v>7</v>
       </c>
@@ -1020,7 +1085,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="I9" s="8"/>
+      <c r="I9" s="9"/>
       <c r="J9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1028,25 +1093,29 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="1"/>
-      <c r="P9" s="11"/>
+      <c r="P9" s="12"/>
       <c r="Q9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
+      <c r="T9" s="5"/>
       <c r="U9" s="1"/>
-      <c r="W9" s="11"/>
+      <c r="W9" s="12"/>
       <c r="X9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
+      <c r="AA9" s="5"/>
       <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
+      <c r="AC9" s="5"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
       <c r="C10" s="2">
         <v>8</v>
       </c>
@@ -1054,7 +1123,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="I10" s="8"/>
+      <c r="I10" s="9"/>
       <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1062,25 +1131,29 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="P10" s="11"/>
+      <c r="P10" s="12"/>
       <c r="Q10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="W10" s="11"/>
+      <c r="W10" s="12"/>
       <c r="X10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+      <c r="AC10" s="5"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
       <c r="C11" s="2">
         <v>9</v>
       </c>
@@ -1088,7 +1161,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="I11" s="8"/>
+      <c r="I11" s="9"/>
       <c r="J11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1096,15 +1169,15 @@
       <c r="L11" s="5"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="P11" s="11"/>
+      <c r="P11" s="12"/>
       <c r="Q11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="W11" s="11"/>
+      <c r="W11" s="12"/>
       <c r="X11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1112,9 +1185,13 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
       <c r="C12" s="2">
         <v>10</v>
       </c>
@@ -1122,7 +1199,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="I12" s="8"/>
+      <c r="I12" s="9"/>
       <c r="J12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1130,25 +1207,29 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="P12" s="11"/>
+      <c r="P12" s="12"/>
       <c r="Q12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
       <c r="U12" s="1"/>
-      <c r="W12" s="11"/>
+      <c r="W12" s="12"/>
       <c r="X12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
+      <c r="AC12" s="5"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
       <c r="C13" s="2">
         <v>11</v>
       </c>
@@ -1156,7 +1237,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="I13" s="8"/>
+      <c r="I13" s="9"/>
       <c r="J13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1164,25 +1245,29 @@
       <c r="L13" s="5"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="P13" s="11"/>
+      <c r="P13" s="12"/>
       <c r="Q13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
-      <c r="W13" s="11"/>
+      <c r="W13" s="12"/>
       <c r="X13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
+      <c r="Z13" s="5"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
+      <c r="AC13" s="5"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
       <c r="C14" s="2">
         <v>12</v>
       </c>
@@ -1190,7 +1275,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="9"/>
       <c r="J14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1198,15 +1283,15 @@
       <c r="L14" s="5"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="P14" s="11"/>
+      <c r="P14" s="12"/>
       <c r="Q14" s="2" t="s">
         <v>37</v>
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="W14" s="11"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="W14" s="12"/>
       <c r="X14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1214,9 +1299,13 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="15"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
       <c r="C15" s="2">
         <v>13</v>
       </c>
@@ -1224,7 +1313,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="I15" s="8"/>
+      <c r="I15" s="9"/>
       <c r="J15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1232,25 +1321,29 @@
       <c r="L15" s="5"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="P15" s="11"/>
+      <c r="P15" s="12"/>
       <c r="Q15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
+      <c r="S15" s="5"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="2" t="s">
+      <c r="W15" s="12"/>
+      <c r="X15" s="16" t="s">
         <v>61</v>
       </c>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B16" s="7"/>
       <c r="C16" s="2">
         <v>14</v>
       </c>
@@ -1258,7 +1351,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="I16" s="8"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1266,15 +1359,15 @@
       <c r="L16" s="5"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="P16" s="11"/>
+      <c r="P16" s="12"/>
       <c r="Q16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R16" s="1"/>
+      <c r="R16" s="5"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-      <c r="W16" s="11"/>
+      <c r="W16" s="12"/>
       <c r="X16" s="2" t="s">
         <v>62</v>
       </c>
@@ -1282,290 +1375,366 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="I17" s="8"/>
-      <c r="J17" s="13" t="s">
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="1"/>
+    </row>
+    <row r="17" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I17" s="9"/>
+      <c r="J17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="1"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="13" t="s">
+      <c r="P17" s="12"/>
+      <c r="Q17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="R17" s="1"/>
+      <c r="R17" s="5"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="13" t="s">
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="Y17" s="1"/>
+      <c r="Y17" s="5"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="I18" s="8"/>
-      <c r="J18" s="13" t="s">
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+    </row>
+    <row r="18" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I18" s="9"/>
+      <c r="J18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="5"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="13" t="s">
+      <c r="P18" s="12"/>
+      <c r="Q18" s="6" t="s">
         <v>41</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+      <c r="S18" s="5"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="13" t="s">
+      <c r="W18" s="12"/>
+      <c r="X18" s="6" t="s">
         <v>64</v>
       </c>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
+      <c r="AA18" s="5"/>
       <c r="AB18" s="1"/>
-    </row>
-    <row r="19" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="I19" s="8"/>
-      <c r="J19" s="13" t="s">
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+    </row>
+    <row r="19" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I19" s="9"/>
+      <c r="J19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="1"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="13" t="s">
+      <c r="P19" s="12"/>
+      <c r="Q19" s="6" t="s">
         <v>42</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="S19" s="5"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="13" t="s">
+      <c r="W19" s="12"/>
+      <c r="X19" s="6" t="s">
         <v>65</v>
       </c>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
-    </row>
-    <row r="20" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="I20" s="9"/>
-      <c r="J20" s="13" t="s">
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="15"/>
+      <c r="AF19" s="1"/>
+    </row>
+    <row r="20" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="I20" s="10"/>
+      <c r="J20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="5"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="13" t="s">
+      <c r="P20" s="12"/>
+      <c r="Q20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="R20" s="1"/>
+      <c r="R20" s="5"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="13" t="s">
+      <c r="W20" s="12"/>
+      <c r="X20" s="6" t="s">
         <v>66</v>
       </c>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
-    </row>
-    <row r="21" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="P21" s="11"/>
-      <c r="Q21" s="13" t="s">
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="15"/>
+    </row>
+    <row r="21" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="P21" s="12"/>
+      <c r="Q21" s="6" t="s">
         <v>44</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
+      <c r="S21" s="5"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="13" t="s">
+      <c r="W21" s="12"/>
+      <c r="X21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
-    </row>
-    <row r="22" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="P22" s="11"/>
-      <c r="Q22" s="13" t="s">
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="15"/>
+      <c r="AF21" s="15"/>
+    </row>
+    <row r="22" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="P22" s="12"/>
+      <c r="Q22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="13" t="s">
+      <c r="W22" s="12"/>
+      <c r="X22" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="Y22" s="1"/>
+      <c r="Y22" s="15"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
-    </row>
-    <row r="23" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="P23" s="11"/>
-      <c r="Q23" s="13" t="s">
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+    </row>
+    <row r="23" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="P23" s="12"/>
+      <c r="Q23" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="13" t="s">
+      <c r="W23" s="12"/>
+      <c r="X23" s="6" t="s">
         <v>69</v>
       </c>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
-    </row>
-    <row r="24" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="P24" s="11"/>
-      <c r="Q24" s="13" t="s">
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="15"/>
+    </row>
+    <row r="24" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="P24" s="12"/>
+      <c r="Q24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R24" s="1"/>
+      <c r="R24" s="5"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="13" t="s">
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="W24" s="12"/>
+      <c r="X24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="Y24" s="1"/>
+      <c r="Y24" s="5"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
-    </row>
-    <row r="25" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="P25" s="12"/>
-      <c r="Q25" s="13" t="s">
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="1"/>
+    </row>
+    <row r="25" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="P25" s="13"/>
+      <c r="Q25" s="6" t="s">
         <v>48</v>
       </c>
       <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
+      <c r="S25" s="5"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="13" t="s">
+      <c r="W25" s="12"/>
+      <c r="X25" s="6" t="s">
         <v>71</v>
       </c>
       <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
+      <c r="Z25" s="5"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
-    </row>
-    <row r="26" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="W26" s="11"/>
-      <c r="X26" s="13" t="s">
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="15"/>
+      <c r="AF25" s="15"/>
+    </row>
+    <row r="26" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="W26" s="12"/>
+      <c r="X26" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="Y26" s="1"/>
+      <c r="Y26" s="5"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
-    </row>
-    <row r="27" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="W27" s="11"/>
-      <c r="X27" s="13" t="s">
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="15"/>
+      <c r="AF26" s="1"/>
+    </row>
+    <row r="27" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="W27" s="12"/>
+      <c r="X27" s="6" t="s">
         <v>73</v>
       </c>
       <c r="Y27" s="1"/>
-      <c r="Z27" s="1"/>
+      <c r="Z27" s="5"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
-    </row>
-    <row r="28" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="W28" s="11"/>
-      <c r="X28" s="13" t="s">
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+    </row>
+    <row r="28" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="W28" s="12"/>
+      <c r="X28" s="17" t="s">
         <v>74</v>
       </c>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
-    </row>
-    <row r="29" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="W29" s="11"/>
-      <c r="X29" s="13" t="s">
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+    </row>
+    <row r="29" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="W29" s="12"/>
+      <c r="X29" s="6" t="s">
         <v>75</v>
       </c>
       <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="Z29" s="5"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
-    </row>
-    <row r="30" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="W30" s="11"/>
-      <c r="X30" s="13" t="s">
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+    </row>
+    <row r="30" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="W30" s="12"/>
+      <c r="X30" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="Y30" s="1"/>
+      <c r="Y30" s="5"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
-    </row>
-    <row r="31" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="W31" s="11"/>
-      <c r="X31" s="13" t="s">
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="15"/>
+    </row>
+    <row r="31" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="W31" s="12"/>
+      <c r="X31" s="6" t="s">
         <v>77</v>
       </c>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
-    </row>
-    <row r="32" spans="9:28" x14ac:dyDescent="0.25">
-      <c r="W32" s="11"/>
-      <c r="X32" s="13" t="s">
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="15"/>
+      <c r="AF31" s="1"/>
+    </row>
+    <row r="32" spans="9:32" x14ac:dyDescent="0.3">
+      <c r="W32" s="12"/>
+      <c r="X32" s="6" t="s">
         <v>78</v>
       </c>
       <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
+      <c r="Z32" s="5"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
-    </row>
-    <row r="33" spans="23:28" x14ac:dyDescent="0.25">
-      <c r="W33" s="11"/>
-      <c r="X33" s="13" t="s">
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+    </row>
+    <row r="33" spans="23:32" x14ac:dyDescent="0.3">
+      <c r="W33" s="12"/>
+      <c r="X33" s="6" t="s">
         <v>79</v>
       </c>
       <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
+      <c r="Z33" s="5"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
-    </row>
-    <row r="34" spans="23:28" x14ac:dyDescent="0.25">
-      <c r="W34" s="12"/>
-      <c r="X34" s="13" t="s">
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
+    </row>
+    <row r="34" spans="23:32" x14ac:dyDescent="0.3">
+      <c r="W34" s="13"/>
+      <c r="X34" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="Y34" s="1"/>
+      <c r="Y34" s="5"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="15"/>
+      <c r="AF34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1575,5 +1744,6 @@
     <mergeCell ref="W3:W34"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding test cases for banco
</commit_message>
<xml_diff>
--- a/Grafo/doc/casos de teste palindromo.xlsx
+++ b/Grafo/doc/casos de teste palindromo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\workspace\ProjTesteSoftware\Grafo\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UFRJ\ProjTesteSoftware\Grafo\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t>CT1</t>
   </si>
@@ -267,35 +267,16 @@
   </si>
   <si>
     <t>(10, 7, 8, 10)</t>
-  </si>
-  <si>
-    <t>CT5</t>
-  </si>
-  <si>
-    <t>CT6</t>
-  </si>
-  <si>
-    <t>CT7</t>
-  </si>
-  <si>
-    <t>CT8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -392,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -401,9 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -425,12 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -747,30 +720,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:AF34"/>
+  <dimension ref="B2:AB34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AD1:AF1"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.88671875" customWidth="1"/>
-    <col min="24" max="24" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="21" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" customWidth="1"/>
+    <col min="24" max="24" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="4.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
@@ -827,21 +798,9 @@
       <c r="AB2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD2" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE2" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF2" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+    </row>
+    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2">
@@ -851,7 +810,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -861,17 +820,17 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
       <c r="U3" s="1"/>
-      <c r="W3" s="11" t="s">
+      <c r="W3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="X3" s="2" t="s">
@@ -879,15 +838,11 @@
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="5"/>
+      <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-    </row>
-    <row r="4" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
+    </row>
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
       <c r="C4" s="2">
         <v>2</v>
       </c>
@@ -895,7 +850,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="I4" s="9"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="2" t="s">
         <v>9</v>
       </c>
@@ -903,29 +858,25 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="1"/>
-      <c r="P4" s="12"/>
+      <c r="P4" s="11"/>
       <c r="Q4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-      <c r="U4" s="5"/>
-      <c r="W4" s="12"/>
+      <c r="U4" s="1"/>
+      <c r="W4" s="11"/>
       <c r="X4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-    </row>
-    <row r="5" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B5" s="7"/>
+    </row>
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
       <c r="C5" s="2">
         <v>3</v>
       </c>
@@ -933,7 +884,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="1"/>
-      <c r="I5" s="9"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="2" t="s">
         <v>10</v>
       </c>
@@ -941,29 +892,25 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="16" t="s">
+      <c r="W5" s="11"/>
+      <c r="X5" s="2" t="s">
         <v>51</v>
       </c>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-    </row>
-    <row r="6" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
+    </row>
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
       <c r="C6" s="2">
         <v>4</v>
       </c>
@@ -971,7 +918,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="I6" s="9"/>
+      <c r="I6" s="8"/>
       <c r="J6" s="2" t="s">
         <v>11</v>
       </c>
@@ -979,29 +926,25 @@
       <c r="L6" s="5"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-      <c r="P6" s="12"/>
+      <c r="P6" s="11"/>
       <c r="Q6" s="2" t="s">
         <v>29</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="5"/>
+      <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="16" t="s">
+      <c r="W6" s="11"/>
+      <c r="X6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-    </row>
-    <row r="7" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
+    </row>
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
       <c r="C7" s="2">
         <v>5</v>
       </c>
@@ -1009,7 +952,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="1"/>
-      <c r="I7" s="9"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1017,29 +960,25 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="1"/>
-      <c r="P7" s="12"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="16" t="s">
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-    </row>
-    <row r="8" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
+    </row>
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
       <c r="C8" s="2">
         <v>6</v>
       </c>
@@ -1047,7 +986,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="I8" s="9"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1055,29 +994,25 @@
       <c r="L8" s="5"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="P8" s="12"/>
+      <c r="P8" s="11"/>
       <c r="Q8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="W8" s="12"/>
+      <c r="W8" s="11"/>
       <c r="X8" s="2" t="s">
         <v>54</v>
       </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-    </row>
-    <row r="9" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B9" s="7"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
       <c r="C9" s="2">
         <v>7</v>
       </c>
@@ -1085,7 +1020,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="I9" s="9"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1093,29 +1028,25 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="1"/>
-      <c r="P9" s="12"/>
+      <c r="P9" s="11"/>
       <c r="Q9" s="2" t="s">
         <v>32</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="5"/>
+      <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="W9" s="12"/>
+      <c r="W9" s="11"/>
       <c r="X9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="5"/>
+      <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-    </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
+    </row>
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
       <c r="C10" s="2">
         <v>8</v>
       </c>
@@ -1123,7 +1054,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="I10" s="9"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1131,29 +1062,25 @@
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
-      <c r="P10" s="12"/>
+      <c r="P10" s="11"/>
       <c r="Q10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="W10" s="12"/>
+      <c r="W10" s="11"/>
       <c r="X10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-    </row>
-    <row r="11" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
+    </row>
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
       <c r="C11" s="2">
         <v>9</v>
       </c>
@@ -1161,7 +1088,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="I11" s="9"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1169,15 +1096,15 @@
       <c r="L11" s="5"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-      <c r="P11" s="12"/>
+      <c r="P11" s="11"/>
       <c r="Q11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="W11" s="12"/>
+      <c r="W11" s="11"/>
       <c r="X11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1185,13 +1112,9 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
-      <c r="AC11" s="15"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-    </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
       <c r="C12" s="2">
         <v>10</v>
       </c>
@@ -1199,7 +1122,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="I12" s="9"/>
+      <c r="I12" s="8"/>
       <c r="J12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1207,29 +1130,25 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
-      <c r="P12" s="12"/>
+      <c r="P12" s="11"/>
       <c r="Q12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
       <c r="U12" s="1"/>
-      <c r="W12" s="12"/>
+      <c r="W12" s="11"/>
       <c r="X12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
-    </row>
-    <row r="13" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B13" s="6"/>
       <c r="C13" s="2">
         <v>11</v>
       </c>
@@ -1237,7 +1156,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="I13" s="9"/>
+      <c r="I13" s="8"/>
       <c r="J13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1245,29 +1164,25 @@
       <c r="L13" s="5"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
-      <c r="P13" s="12"/>
+      <c r="P13" s="11"/>
       <c r="Q13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
-      <c r="W13" s="12"/>
+      <c r="W13" s="11"/>
       <c r="X13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="Y13" s="1"/>
-      <c r="Z13" s="5"/>
+      <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
-    </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+    </row>
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B14" s="6"/>
       <c r="C14" s="2">
         <v>12</v>
       </c>
@@ -1275,7 +1190,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="I14" s="9"/>
+      <c r="I14" s="8"/>
       <c r="J14" s="2" t="s">
         <v>19</v>
       </c>
@@ -1283,15 +1198,15 @@
       <c r="L14" s="5"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-      <c r="P14" s="12"/>
+      <c r="P14" s="11"/>
       <c r="Q14" s="2" t="s">
         <v>37</v>
       </c>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
-      <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-      <c r="W14" s="12"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="W14" s="11"/>
       <c r="X14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1299,13 +1214,9 @@
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
-    </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
       <c r="C15" s="2">
         <v>13</v>
       </c>
@@ -1313,7 +1224,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="I15" s="9"/>
+      <c r="I15" s="8"/>
       <c r="J15" s="2" t="s">
         <v>20</v>
       </c>
@@ -1321,29 +1232,25 @@
       <c r="L15" s="5"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
-      <c r="P15" s="12"/>
+      <c r="P15" s="11"/>
       <c r="Q15" s="2" t="s">
         <v>38</v>
       </c>
       <c r="R15" s="1"/>
-      <c r="S15" s="5"/>
+      <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="W15" s="12"/>
-      <c r="X15" s="16" t="s">
+      <c r="W15" s="11"/>
+      <c r="X15" s="2" t="s">
         <v>61</v>
       </c>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
-    </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
       <c r="C16" s="2">
         <v>14</v>
       </c>
@@ -1351,7 +1258,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="2" t="s">
         <v>21</v>
       </c>
@@ -1359,15 +1266,15 @@
       <c r="L16" s="5"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
-      <c r="P16" s="12"/>
+      <c r="P16" s="11"/>
       <c r="Q16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="R16" s="5"/>
+      <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-      <c r="W16" s="12"/>
+      <c r="W16" s="11"/>
       <c r="X16" s="2" t="s">
         <v>62</v>
       </c>
@@ -1375,366 +1282,290 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="15"/>
-      <c r="AF16" s="1"/>
-    </row>
-    <row r="17" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I17" s="9"/>
-      <c r="J17" s="6" t="s">
+    </row>
+    <row r="17" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I17" s="8"/>
+      <c r="J17" s="13" t="s">
         <v>22</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="1"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="6" t="s">
+      <c r="P17" s="11"/>
+      <c r="Q17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="R17" s="5"/>
+      <c r="R17" s="1"/>
       <c r="S17" s="1"/>
-      <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="6" t="s">
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="Y17" s="5"/>
+      <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="1"/>
-    </row>
-    <row r="18" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I18" s="9"/>
-      <c r="J18" s="6" t="s">
+    </row>
+    <row r="18" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I18" s="8"/>
+      <c r="J18" s="13" t="s">
         <v>23</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="5"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="6" t="s">
+      <c r="P18" s="11"/>
+      <c r="Q18" s="13" t="s">
         <v>41</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="5"/>
+      <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="6" t="s">
+      <c r="W18" s="11"/>
+      <c r="X18" s="13" t="s">
         <v>64</v>
       </c>
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="5"/>
+      <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
-    </row>
-    <row r="19" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I19" s="9"/>
-      <c r="J19" s="6" t="s">
+    </row>
+    <row r="19" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I19" s="8"/>
+      <c r="J19" s="13" t="s">
         <v>24</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="1"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="6" t="s">
+      <c r="P19" s="11"/>
+      <c r="Q19" s="13" t="s">
         <v>42</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="5"/>
+      <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="6" t="s">
+      <c r="W19" s="11"/>
+      <c r="X19" s="13" t="s">
         <v>65</v>
       </c>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="1"/>
-    </row>
-    <row r="20" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="I20" s="10"/>
-      <c r="J20" s="6" t="s">
+    </row>
+    <row r="20" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="I20" s="9"/>
+      <c r="J20" s="13" t="s">
         <v>25</v>
       </c>
       <c r="K20" s="1"/>
       <c r="L20" s="5"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="6" t="s">
+      <c r="P20" s="11"/>
+      <c r="Q20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="R20" s="5"/>
+      <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
-      <c r="W20" s="12"/>
-      <c r="X20" s="6" t="s">
+      <c r="W20" s="11"/>
+      <c r="X20" s="13" t="s">
         <v>66</v>
       </c>
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
-      <c r="AE20" s="1"/>
-      <c r="AF20" s="15"/>
-    </row>
-    <row r="21" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="P21" s="12"/>
-      <c r="Q21" s="6" t="s">
+    </row>
+    <row r="21" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="P21" s="11"/>
+      <c r="Q21" s="13" t="s">
         <v>44</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="S21" s="5"/>
+      <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="6" t="s">
+      <c r="W21" s="11"/>
+      <c r="X21" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="15"/>
-    </row>
-    <row r="22" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="P22" s="12"/>
-      <c r="Q22" s="6" t="s">
+    </row>
+    <row r="22" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="P22" s="11"/>
+      <c r="Q22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="6" t="s">
+      <c r="W22" s="11"/>
+      <c r="X22" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y22" s="15"/>
+      <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
-      <c r="AC22" s="5"/>
-      <c r="AD22" s="1"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="15"/>
-    </row>
-    <row r="23" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="P23" s="12"/>
-      <c r="Q23" s="6" t="s">
+    </row>
+    <row r="23" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="P23" s="11"/>
+      <c r="Q23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="6" t="s">
+      <c r="W23" s="11"/>
+      <c r="X23" s="13" t="s">
         <v>69</v>
       </c>
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-      <c r="AE23" s="1"/>
-      <c r="AF23" s="15"/>
-    </row>
-    <row r="24" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="P24" s="12"/>
-      <c r="Q24" s="6" t="s">
+    </row>
+    <row r="24" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="P24" s="11"/>
+      <c r="Q24" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="R24" s="5"/>
+      <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="6" t="s">
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="Y24" s="5"/>
+      <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
-      <c r="AE24" s="15"/>
-      <c r="AF24" s="1"/>
-    </row>
-    <row r="25" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="P25" s="13"/>
-      <c r="Q25" s="6" t="s">
+    </row>
+    <row r="25" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="P25" s="12"/>
+      <c r="Q25" s="13" t="s">
         <v>48</v>
       </c>
       <c r="R25" s="1"/>
-      <c r="S25" s="5"/>
+      <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="6" t="s">
+      <c r="W25" s="11"/>
+      <c r="X25" s="13" t="s">
         <v>71</v>
       </c>
       <c r="Y25" s="1"/>
-      <c r="Z25" s="5"/>
+      <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="1"/>
-      <c r="AE25" s="15"/>
-      <c r="AF25" s="15"/>
-    </row>
-    <row r="26" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="W26" s="12"/>
-      <c r="X26" s="6" t="s">
+    </row>
+    <row r="26" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="W26" s="11"/>
+      <c r="X26" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="Y26" s="5"/>
+      <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
       <c r="AA26" s="1"/>
       <c r="AB26" s="1"/>
-      <c r="AC26" s="1"/>
-      <c r="AD26" s="1"/>
-      <c r="AE26" s="15"/>
-      <c r="AF26" s="1"/>
-    </row>
-    <row r="27" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="W27" s="12"/>
-      <c r="X27" s="6" t="s">
+    </row>
+    <row r="27" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="W27" s="11"/>
+      <c r="X27" s="13" t="s">
         <v>73</v>
       </c>
       <c r="Y27" s="1"/>
-      <c r="Z27" s="5"/>
+      <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
-      <c r="AC27" s="1"/>
-      <c r="AD27" s="1"/>
-      <c r="AE27" s="1"/>
-      <c r="AF27" s="1"/>
-    </row>
-    <row r="28" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="W28" s="12"/>
-      <c r="X28" s="17" t="s">
+    </row>
+    <row r="28" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="W28" s="11"/>
+      <c r="X28" s="13" t="s">
         <v>74</v>
       </c>
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
-      <c r="AC28" s="1"/>
-      <c r="AD28" s="1"/>
-      <c r="AE28" s="1"/>
-      <c r="AF28" s="1"/>
-    </row>
-    <row r="29" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="W29" s="12"/>
-      <c r="X29" s="6" t="s">
+    </row>
+    <row r="29" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="W29" s="11"/>
+      <c r="X29" s="13" t="s">
         <v>75</v>
       </c>
       <c r="Y29" s="1"/>
-      <c r="Z29" s="5"/>
+      <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="1"/>
-      <c r="AE29" s="1"/>
-      <c r="AF29" s="1"/>
-    </row>
-    <row r="30" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="W30" s="12"/>
-      <c r="X30" s="6" t="s">
+    </row>
+    <row r="30" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="W30" s="11"/>
+      <c r="X30" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="Y30" s="5"/>
+      <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-      <c r="AE30" s="1"/>
-      <c r="AF30" s="15"/>
-    </row>
-    <row r="31" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="W31" s="12"/>
-      <c r="X31" s="6" t="s">
+    </row>
+    <row r="31" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="W31" s="11"/>
+      <c r="X31" s="13" t="s">
         <v>77</v>
       </c>
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-      <c r="AE31" s="15"/>
-      <c r="AF31" s="1"/>
-    </row>
-    <row r="32" spans="9:32" x14ac:dyDescent="0.3">
-      <c r="W32" s="12"/>
-      <c r="X32" s="6" t="s">
+    </row>
+    <row r="32" spans="9:28" x14ac:dyDescent="0.25">
+      <c r="W32" s="11"/>
+      <c r="X32" s="13" t="s">
         <v>78</v>
       </c>
       <c r="Y32" s="1"/>
-      <c r="Z32" s="5"/>
+      <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
       <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-      <c r="AE32" s="1"/>
-      <c r="AF32" s="1"/>
-    </row>
-    <row r="33" spans="23:32" x14ac:dyDescent="0.3">
-      <c r="W33" s="12"/>
-      <c r="X33" s="6" t="s">
+    </row>
+    <row r="33" spans="23:28" x14ac:dyDescent="0.25">
+      <c r="W33" s="11"/>
+      <c r="X33" s="13" t="s">
         <v>79</v>
       </c>
       <c r="Y33" s="1"/>
-      <c r="Z33" s="5"/>
+      <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-      <c r="AE33" s="1"/>
-      <c r="AF33" s="1"/>
-    </row>
-    <row r="34" spans="23:32" x14ac:dyDescent="0.3">
-      <c r="W34" s="13"/>
-      <c r="X34" s="6" t="s">
+    </row>
+    <row r="34" spans="23:28" x14ac:dyDescent="0.25">
+      <c r="W34" s="12"/>
+      <c r="X34" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="Y34" s="5"/>
+      <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1"/>
-      <c r="AE34" s="15"/>
-      <c r="AF34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1744,6 +1575,5 @@
     <mergeCell ref="W3:W34"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>